<commit_message>
1. modify uart communication bug
</commit_message>
<xml_diff>
--- a/Document/uart protocol.xlsx
+++ b/Document/uart protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\project\ChargingCase\ChargingCase_CMS32L051\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D71B9A-B7FA-42CA-8E5D-56F1C1644D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA5CBB5-6F02-4915-B084-934F42522926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5690" yWindow="600" windowWidth="13510" windowHeight="9760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>0x5a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,38 +141,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">lcd data update </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lcd data update enable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lcd data update ack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cmd:  0x03</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>picture index: 1~(total picture num)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max bytes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>max bytes:  64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cmd: 0x84</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">picture width </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -202,6 +182,98 @@
   </si>
   <si>
     <t>ack/nack: 0x01-&gt;ack, 0x0-&gt;nack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fw data update enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">fw length </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">fw length: </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">lcd data send </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fw data send</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offset addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">offset addr </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buf[0]…buf[max]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offset addr: 0~65536(2 bytes)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0~65536(2 bytes)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lcd  ack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fw  ack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get fw version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">send fw version </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minor version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>build version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>major version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x09</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -253,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -263,11 +335,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -551,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -571,19 +644,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -699,7 +772,7 @@
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -716,13 +789,13 @@
         <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -735,22 +808,22 @@
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -767,32 +840,34 @@
         <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -809,47 +884,225 @@
         <v>4</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
+    <mergeCell ref="A48:XFD48"/>
+    <mergeCell ref="A49:XFD49"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="A9:XFD9"/>
+    <mergeCell ref="A10:XFD10"/>
+    <mergeCell ref="A11:XFD11"/>
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A18:XFD18"/>
+    <mergeCell ref="A20:XFD20"/>
+    <mergeCell ref="A21:XFD21"/>
+    <mergeCell ref="A25:XFD25"/>
+    <mergeCell ref="A27:XFD27"/>
+    <mergeCell ref="A12:XFD12"/>
+    <mergeCell ref="A13:XFD13"/>
+    <mergeCell ref="A14:XFD14"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="A16:XFD16"/>
     <mergeCell ref="A28:XFD28"/>
     <mergeCell ref="A29:XFD29"/>
     <mergeCell ref="A34:XFD34"/>
     <mergeCell ref="A33:XFD33"/>
     <mergeCell ref="A22:XFD22"/>
     <mergeCell ref="A23:XFD23"/>
-    <mergeCell ref="A12:XFD12"/>
-    <mergeCell ref="A13:XFD13"/>
-    <mergeCell ref="A14:XFD14"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A18:XFD18"/>
-    <mergeCell ref="A20:XFD20"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A25:XFD25"/>
-    <mergeCell ref="A27:XFD27"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A8:XFD8"/>
-    <mergeCell ref="A9:XFD9"/>
-    <mergeCell ref="A10:XFD10"/>
-    <mergeCell ref="A11:XFD11"/>
-    <mergeCell ref="A2:XFD2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
continue to debug upgrade function
</commit_message>
<xml_diff>
--- a/Document/uart protocol.xlsx
+++ b/Document/uart protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\project\ChargingCase\ChargingCase_CMS32L051\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA5CBB5-6F02-4915-B084-934F42522926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC35E70-867A-4DEB-A311-1DB980B16E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5690" yWindow="600" windowWidth="13510" windowHeight="9760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
   <si>
     <t>0x5a</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -185,10 +185,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>fw data update enable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">fw length </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,10 +253,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">send fw version </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>minor version</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,6 +266,26 @@
   </si>
   <si>
     <t>cmd: 0x09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fw erase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fw checksum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fw checksum : fw check sum,  CRC-16/CCITT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">set fw version </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd: 0x89</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -325,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -337,10 +349,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -624,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -655,8 +668,8 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -725,53 +738,53 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -801,29 +814,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>44</v>
+    <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -840,34 +853,34 @@
         <v>4</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+    <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -891,22 +904,22 @@
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+    <row r="33" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>0</v>
       </c>
@@ -920,32 +933,32 @@
         <v>4</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
       <c r="B39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -959,35 +972,36 @@
         <v>4</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="5" t="s">
+    <row r="45" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -996,30 +1010,29 @@
       <c r="D47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F47" s="1" t="s">
+      <c r="E47" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>0</v>
       </c>
@@ -1033,54 +1046,98 @@
         <v>4</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="F61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H56" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>62</v>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A48:XFD48"/>
-    <mergeCell ref="A49:XFD49"/>
+    <mergeCell ref="A15:XFD15"/>
+    <mergeCell ref="A16:XFD16"/>
+    <mergeCell ref="A28:XFD28"/>
+    <mergeCell ref="A29:XFD29"/>
+    <mergeCell ref="A34:XFD34"/>
+    <mergeCell ref="A33:XFD33"/>
+    <mergeCell ref="A22:XFD22"/>
+    <mergeCell ref="A23:XFD23"/>
+    <mergeCell ref="A53:XFD53"/>
+    <mergeCell ref="A54:XFD54"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A8:XFD8"/>
     <mergeCell ref="A9:XFD9"/>
@@ -1095,14 +1152,6 @@
     <mergeCell ref="A12:XFD12"/>
     <mergeCell ref="A13:XFD13"/>
     <mergeCell ref="A14:XFD14"/>
-    <mergeCell ref="A15:XFD15"/>
-    <mergeCell ref="A16:XFD16"/>
-    <mergeCell ref="A28:XFD28"/>
-    <mergeCell ref="A29:XFD29"/>
-    <mergeCell ref="A34:XFD34"/>
-    <mergeCell ref="A33:XFD33"/>
-    <mergeCell ref="A22:XFD22"/>
-    <mergeCell ref="A23:XFD23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>